<commit_message>
ITF CSVs, IF implemented, fixes
</commit_message>
<xml_diff>
--- a/MRK_Full Trrade.xlsx
+++ b/MRK_Full Trrade.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MarcbookPro/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MarcbookPro/Projects/PriceAction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D04C625-54EB-614A-9614-429B7127C039}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFF928B-4B92-E842-A2C4-1736CB43BBE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_mrk" sheetId="3" r:id="rId1"/>
@@ -5105,8 +5105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11785,8 +11785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A348BFB5-915C-4506-AF54-FE1B1981CB47}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11877,7 +11877,7 @@
         <v>38</v>
       </c>
       <c r="B11" s="16">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -12014,7 +12014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20076C46-A197-4871-A4FF-9484FF203543}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>